<commit_message>
Update Toby's assessment of false positives by all methods.
</commit_message>
<xml_diff>
--- a/crowd_only/data/final_eval/analysis/testset_all_predictions_agree_false_positives.xlsx
+++ b/crowd_only/data/final_eval/analysis/testset_all_predictions_agree_false_positives.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -602,7 +602,7 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N3" activeCellId="0" sqref="N3"/>
+      <selection pane="topLeft" activeCell="O8" activeCellId="0" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -611,9 +611,10 @@
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="14.9030612244898"/>
     <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.72959183673469"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.1020408163265"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.9081632653061"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.0459183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.1275510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Add Andrew's and Ben's assessments of the shared false positives.
Added Andrew's and Ben's assessments of the relations which were all
predicted by the three methods but which were considered false positives
by the gold standard.
</commit_message>
<xml_diff>
--- a/crowd_only/data/final_eval/analysis/testset_all_predictions_agree_false_positives.xlsx
+++ b/crowd_only/data/final_eval/analysis/testset_all_predictions_agree_false_positives.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="176">
   <si>
     <t>pmid</t>
   </si>
@@ -50,10 +50,22 @@
     <t>rel_origin</t>
   </si>
   <si>
+    <t>toby_gold_error</t>
+  </si>
+  <si>
+    <t>ben_gold_error</t>
+  </si>
+  <si>
+    <t>andrew_gold_error</t>
+  </si>
+  <si>
+    <t>final_gold_error</t>
+  </si>
+  <si>
     <t>covered_by_guidelines</t>
   </si>
   <si>
-    <t>gold_error</t>
+    <t>ben_comments</t>
   </si>
   <si>
     <t>error_reason</t>
@@ -98,30 +110,39 @@
     <t>cid_relation</t>
   </si>
   <si>
+    <t>missing_relation</t>
+  </si>
+  <si>
+    <t>Text states two specific examples of embryopathy which were used instead. Not MeSH filterable.</t>
+  </si>
+  <si>
+    <t>MESH:D003676</t>
+  </si>
+  <si>
+    <t>MESH:D058186</t>
+  </si>
+  <si>
+    <t>http://ncbi.nlm.nih.gov/pubmed/?term=1289188</t>
+  </si>
+  <si>
+    <t>https://crowdflower.com/jobs/767262/units/773932515</t>
+  </si>
+  <si>
+    <t>This is the overdose situation again.  Note that the reader would need to see the whole abstract to know that.</t>
+  </si>
+  <si>
     <t>hierarchy_error</t>
   </si>
   <si>
-    <t>Text states two specific examples of embryopathy which were used instead. Not MeSH filterable.</t>
-  </si>
-  <si>
-    <t>MESH:D003676</t>
-  </si>
-  <si>
-    <t>MESH:D058186</t>
-  </si>
-  <si>
-    <t>http://ncbi.nlm.nih.gov/pubmed/?term=1289188</t>
-  </si>
-  <si>
-    <t>https://crowdflower.com/jobs/767262/units/773932515</t>
-  </si>
-  <si>
     <t>Gold uses renal insufficiency instead of acute renal failure. However, acute renal failure is actually more specific because it is lower in the MeSH Ontology. Seems like gold is being inconsistent.</t>
   </si>
   <si>
     <t>https://crowdflower.com/jobs/767262/units/773932517</t>
   </si>
   <si>
+    <t>same as above</t>
+  </si>
+  <si>
     <t>MESH:D016595</t>
   </si>
   <si>
@@ -134,6 +155,9 @@
     <t>https://crowdflower.com/jobs/767262/units/773932601</t>
   </si>
   <si>
+    <t>Not a direct assertion, but certainly implied</t>
+  </si>
+  <si>
     <t>not_main_point</t>
   </si>
   <si>
@@ -152,6 +176,9 @@
     <t>https://crowdflower.com/jobs/767262/units/773932662</t>
   </si>
   <si>
+    <t>Not even implied</t>
+  </si>
+  <si>
     <t>The crux here is whether seizures is a different disease than status epilepticus (epileptic seizures follow one another without recovery of consciousness between them). The text seems to use them interchangeably, but also seems to suggest that they are different. The two terms are closely related in the MeSH hierarchy but not direct descendants of one another.</t>
   </si>
   <si>
@@ -164,6 +191,9 @@
     <t>https://crowdflower.com/jobs/767262/units/773932669</t>
   </si>
   <si>
+    <t>seizure induced by drug..  Tought to avoid saying the drug contributes to the disease unless this situation explicitly covered in guidelines</t>
+  </si>
+  <si>
     <t>MESH:D003520</t>
   </si>
   <si>
@@ -185,6 +215,9 @@
     <t>https://crowdflower.com/jobs/767262/units/773932889</t>
   </si>
   <si>
+    <t>Very clear</t>
+  </si>
+  <si>
     <t>Gold seems to have used a less specific disease here (nephrotoxicity) instead of the more specific acute renal failure. MeSH filterable.</t>
   </si>
   <si>
@@ -200,7 +233,7 @@
     <t>https://crowdflower.com/jobs/767262/units/773932950</t>
   </si>
   <si>
-    <t>missing_relation</t>
+    <t>3 out of 4 patients given the drug developed the disease</t>
   </si>
   <si>
     <t>Seems like relation is missing in gold here. The only gold relation is between lidocaine and hypotension, which is using the same sentence as this relation. The text implies that three patients had asystole due to lidocaine, which was severe enough that the patients died.</t>
@@ -221,162 +254,195 @@
     <t>abstract_task</t>
   </si>
   <si>
+    <t>same as above - group a with drug had more of disease</t>
+  </si>
+  <si>
+    <t>Endografine and diatrizoate are annotated as two different things in the gold standard, and the gold uses endografine in the relation to abdominal pain. However, based on the way the text is presented, it seems that endografine and diatrizoate should be used interchangably, since diatrizoate is given in brackets immediately afterwards. Seems like this is a concept disambiguation problem.</t>
+  </si>
+  <si>
+    <t>MESH:D001778</t>
+  </si>
+  <si>
+    <t>http://ncbi.nlm.nih.gov/pubmed/?term=8308951</t>
+  </si>
+  <si>
+    <t>intermediate_agent</t>
+  </si>
+  <si>
+    <t>This is an example of the drug-induced disease disease pattern. Strictly speaking the gold should have included this relation and not the one between warfarin and intercerebral hematoma.</t>
+  </si>
+  <si>
+    <t>MESH:D018170</t>
+  </si>
+  <si>
+    <t>MESH:D003329</t>
+  </si>
+  <si>
+    <t>http://ncbi.nlm.nih.gov/pubmed/?term=9759693</t>
+  </si>
+  <si>
+    <t>https://crowdflower.com/jobs/767262/units/773933474</t>
+  </si>
+  <si>
+    <t>same strucure as above</t>
+  </si>
+  <si>
+    <t>The abstract summarizes the results of other papers as background information, but the main finding of the authors is to describe a new side effect of sumatriptan. The guidelines were not clear how to treat these statements, and therefore sometimes the gold includes the relations, and sometimes it doesn't.</t>
+  </si>
+  <si>
+    <t>MESH:D009203</t>
+  </si>
+  <si>
+    <t>https://crowdflower.com/jobs/767262/units/773933476</t>
+  </si>
+  <si>
+    <t>same sentence as right above</t>
+  </si>
+  <si>
+    <t>MESH:D013411</t>
+  </si>
+  <si>
+    <t>MESH:D051437</t>
+  </si>
+  <si>
+    <t>http://ncbi.nlm.nih.gov/pubmed/?term=10939760</t>
+  </si>
+  <si>
+    <t>https://crowdflower.com/jobs/767262/units/773933603</t>
+  </si>
+  <si>
+    <t>Acute nephrotoxicity is a more specific disease than renal failure and was used by the gold standard instead. MeSH filterable.</t>
+  </si>
+  <si>
+    <t>MESH:D011441</t>
+  </si>
+  <si>
+    <t>MESH:D014657</t>
+  </si>
+  <si>
+    <t>http://ncbi.nlm.nih.gov/pubmed/?term=11380496</t>
+  </si>
+  <si>
+    <t>https://crowdflower.com/jobs/767262/units/773933674</t>
+  </si>
+  <si>
+    <t>helps to read the abstract</t>
+  </si>
+  <si>
+    <t>The abstract begins by saying that previous reports of vasculitis when treated with PTU have occurred, but ends by saying their own results found no link between the two. Guidelines were not clear how internal inconsistencies should be resolved.</t>
+  </si>
+  <si>
+    <t>https://crowdflower.com/jobs/767262/units/773933676</t>
+  </si>
+  <si>
+    <t>https://crowdflower.com/jobs/767262/units/773933679</t>
+  </si>
+  <si>
+    <t>lots from this abstract</t>
+  </si>
+  <si>
+    <t>https://crowdflower.com/jobs/767262/units/773933683</t>
+  </si>
+  <si>
+    <t>again</t>
+  </si>
+  <si>
+    <t>MESH:D003042</t>
+  </si>
+  <si>
+    <t>MESH:D002637</t>
+  </si>
+  <si>
+    <t>http://ncbi.nlm.nih.gov/pubmed/?term=12359538</t>
+  </si>
+  <si>
+    <t>https://crowdflower.com/jobs/767262/units/773933776</t>
+  </si>
+  <si>
+    <t>drug would seem to have caused the disease</t>
+  </si>
+  <si>
+    <t>It is previously known that cocaine causes general chest pain in patients. The authors of the paper wanted to test whether troponin levels could be used as a better diagnostic of myocardial infarction in patients who took cocaine. They found that troponin could be a diagnostic biomarker. The gold used myocardial infarction as the more specific disease. Not MeSH filterable.</t>
+  </si>
+  <si>
+    <t>https://crowdflower.com/jobs/767262/units/773933779</t>
+  </si>
+  <si>
+    <t>https://crowdflower.com/jobs/767262/units/773933781</t>
+  </si>
+  <si>
+    <t>https://crowdflower.com/jobs/767262/units/773933784</t>
+  </si>
+  <si>
+    <t>MESH:D006948</t>
+  </si>
+  <si>
+    <t>http://ncbi.nlm.nih.gov/pubmed/?term=12523489</t>
+  </si>
+  <si>
+    <t>Whether statements stating that a link exists should be included when it is not the main point of the abstract is not clear. Here cocaine was used to cause the hyperactivity in the mouse model, and the authors were testing adenosine receptor agonists for their abilities to reduce locomotor activity.</t>
+  </si>
+  <si>
+    <t>MESH:D000082</t>
+  </si>
+  <si>
+    <t>MESH:D062787</t>
+  </si>
+  <si>
+    <t>http://ncbi.nlm.nih.gov/pubmed/?term=12828076</t>
+  </si>
+  <si>
+    <t>https://crowdflower.com/jobs/767262/units/773933843</t>
+  </si>
+  <si>
+    <t>OVERDOSE</t>
+  </si>
+  <si>
+    <t>The main point of the paper is to determine the role of sFas in acute liver failure. Overuse of paracetamol causes liver failure, and patients with liver failure also have higher sFas levels. Here overdose is a “disease”, but I guess the relation is not included because everything can cause overdose if you take too much of a chemical.</t>
+  </si>
+  <si>
+    <t>https://crowdflower.com/jobs/767262/units/773933846</t>
+  </si>
+  <si>
+    <t>same</t>
+  </si>
+  <si>
+    <t>MESH:D008691</t>
+  </si>
+  <si>
+    <t>MESH:D016171</t>
+  </si>
+  <si>
+    <t>http://ncbi.nlm.nih.gov/pubmed/?term=16801510</t>
+  </si>
+  <si>
+    <t>https://crowdflower.com/jobs/767262/units/773934059</t>
+  </si>
+  <si>
+    <t>but see row 13 and 14 above.  I'd say no in this case because the fraction of cases is so low.</t>
+  </si>
+  <si>
+    <t>low_frequency</t>
+  </si>
+  <si>
+    <t>Text states that six patients receiving methadone presented with torsades de pointes. Text also states that 16 percent of patients receiving methadone developed prolonged QT intervals. Gold treats these two diseases as separate entities, and they are not closely related on MeSH. The effect is small, so maybe that is why the gold did not include this relation.</t>
+  </si>
+  <si>
+    <t>MESH:C004656</t>
+  </si>
+  <si>
+    <t>MESH:D009336</t>
+  </si>
+  <si>
+    <t>http://ncbi.nlm.nih.gov/pubmed/?term=17035713</t>
+  </si>
+  <si>
+    <t>https://crowdflower.com/jobs/767262/units/773934101</t>
+  </si>
+  <si>
     <t>ner_error</t>
   </si>
   <si>
-    <t>Endografine and diatrizoate are annotated as two different things in the gold standard, and the gold uses endografine in the relation to abdominal pain. However, based on the way the text is presented, it seems that endografine and diatrizoate should be used interchangably, since diatrizoate is given in brackets immediately afterwards. Seems like this is a concept disambiguation problem.</t>
-  </si>
-  <si>
-    <t>MESH:D001778</t>
-  </si>
-  <si>
-    <t>http://ncbi.nlm.nih.gov/pubmed/?term=8308951</t>
-  </si>
-  <si>
-    <t>intermediate_agent</t>
-  </si>
-  <si>
-    <t>This is an example of the drug-induced disease disease pattern. Strictly speaking the gold should have included this relation and not the one between warfarin and intercerebral hematoma.</t>
-  </si>
-  <si>
-    <t>MESH:D018170</t>
-  </si>
-  <si>
-    <t>MESH:D003329</t>
-  </si>
-  <si>
-    <t>http://ncbi.nlm.nih.gov/pubmed/?term=9759693</t>
-  </si>
-  <si>
-    <t>https://crowdflower.com/jobs/767262/units/773933474</t>
-  </si>
-  <si>
-    <t>The abstract summarizes the results of other papers as background information, but the main finding of the authors is to describe a new side effect of sumatriptan. The guidelines were not clear how to treat these statements, and therefore sometimes the gold includes the relations, and sometimes it doesn't.</t>
-  </si>
-  <si>
-    <t>MESH:D009203</t>
-  </si>
-  <si>
-    <t>https://crowdflower.com/jobs/767262/units/773933476</t>
-  </si>
-  <si>
-    <t>MESH:D013411</t>
-  </si>
-  <si>
-    <t>MESH:D051437</t>
-  </si>
-  <si>
-    <t>http://ncbi.nlm.nih.gov/pubmed/?term=10939760</t>
-  </si>
-  <si>
-    <t>https://crowdflower.com/jobs/767262/units/773933603</t>
-  </si>
-  <si>
-    <t>Acute nephrotoxicity is a more specific disease than renal failure and was used by the gold standard instead. MeSH filterable.</t>
-  </si>
-  <si>
-    <t>MESH:D011441</t>
-  </si>
-  <si>
-    <t>MESH:D014657</t>
-  </si>
-  <si>
-    <t>http://ncbi.nlm.nih.gov/pubmed/?term=11380496</t>
-  </si>
-  <si>
-    <t>https://crowdflower.com/jobs/767262/units/773933674</t>
-  </si>
-  <si>
-    <t>The abstract begins by saying that previous reports of vasculitis when treated with PTU have occurred, but ends by saying their own results found no link between the two. Guidelines were not clear how internal inconsistencies should be resolved.</t>
-  </si>
-  <si>
-    <t>https://crowdflower.com/jobs/767262/units/773933676</t>
-  </si>
-  <si>
-    <t>https://crowdflower.com/jobs/767262/units/773933679</t>
-  </si>
-  <si>
-    <t>https://crowdflower.com/jobs/767262/units/773933683</t>
-  </si>
-  <si>
-    <t>MESH:D003042</t>
-  </si>
-  <si>
-    <t>MESH:D002637</t>
-  </si>
-  <si>
-    <t>http://ncbi.nlm.nih.gov/pubmed/?term=12359538</t>
-  </si>
-  <si>
-    <t>https://crowdflower.com/jobs/767262/units/773933776</t>
-  </si>
-  <si>
-    <t>It is previously known that cocaine causes general chest pain in patients. The authors of the paper wanted to test whether troponin levels could be used as a better diagnostic of myocardial infarction in patients who took cocaine. They found that troponin could be a diagnostic biomarker. The gold used myocardial infarction as the more specific disease. Not MeSH filterable.</t>
-  </si>
-  <si>
-    <t>https://crowdflower.com/jobs/767262/units/773933779</t>
-  </si>
-  <si>
-    <t>https://crowdflower.com/jobs/767262/units/773933781</t>
-  </si>
-  <si>
-    <t>https://crowdflower.com/jobs/767262/units/773933784</t>
-  </si>
-  <si>
-    <t>MESH:D006948</t>
-  </si>
-  <si>
-    <t>http://ncbi.nlm.nih.gov/pubmed/?term=12523489</t>
-  </si>
-  <si>
-    <t>Whether statements stating that a link exists should be included when it is not the main point of the abstract is not clear. Here cocaine was used to cause the hyperactivity in the mouse model, and the authors were testing adenosine receptor agonists for their abilities to reduce locomotor activity.</t>
-  </si>
-  <si>
-    <t>MESH:D000082</t>
-  </si>
-  <si>
-    <t>MESH:D062787</t>
-  </si>
-  <si>
-    <t>http://ncbi.nlm.nih.gov/pubmed/?term=12828076</t>
-  </si>
-  <si>
-    <t>https://crowdflower.com/jobs/767262/units/773933843</t>
-  </si>
-  <si>
-    <t>The main point of the paper is to determine the role of sFas in acute liver failure. Overuse of paracetamol causes liver failure, and patients with liver failure also have higher sFas levels. Here overdose is a “disease”, but I guess the relation is not included because everything can cause overdose if you take too much of a chemical.</t>
-  </si>
-  <si>
-    <t>https://crowdflower.com/jobs/767262/units/773933846</t>
-  </si>
-  <si>
-    <t>MESH:D008691</t>
-  </si>
-  <si>
-    <t>MESH:D016171</t>
-  </si>
-  <si>
-    <t>http://ncbi.nlm.nih.gov/pubmed/?term=16801510</t>
-  </si>
-  <si>
-    <t>https://crowdflower.com/jobs/767262/units/773934059</t>
-  </si>
-  <si>
-    <t>Text states that six patients receiving methadone presented with torsades de pointes. Text also states that 16 percent of patients receiving methadone developed prolonged QT intervals. Gold treats these two diseases as separate entities, and they are not closely related on MeSH. However, since the two seem to be different diseases, it seems that the gold standard is missing a relation.</t>
-  </si>
-  <si>
-    <t>MESH:C004656</t>
-  </si>
-  <si>
-    <t>MESH:D009336</t>
-  </si>
-  <si>
-    <t>http://ncbi.nlm.nih.gov/pubmed/?term=17035713</t>
-  </si>
-  <si>
-    <t>https://crowdflower.com/jobs/767262/units/773934101</t>
-  </si>
-  <si>
     <t>Necrosis is marked as a disease, but in context is really part of necrosis markers, which is a class of chemicals.</t>
   </si>
   <si>
@@ -392,6 +458,9 @@
     <t>https://crowdflower.com/jobs/767262/units/773932376</t>
   </si>
   <si>
+    <t>weak, but that is what it says</t>
+  </si>
+  <si>
     <t>Text does suggest that cocaine is related to cardiac arrhythmia, but it seems like this is not the main point of the paper, and as such the relation was ignored.</t>
   </si>
   <si>
@@ -416,7 +485,7 @@
     <t>https://crowdflower.com/jobs/767262/units/773931934</t>
   </si>
   <si>
-    <t>Pethidine works through an intermediate metabolite norpethidine. Not clear based on instructions whether this should be considered true or not.</t>
+    <t>Pethidine works through an intermediate metabolite norpethidine. Guidelines are ambiguous as to whether these kinds of relations should be included.</t>
   </si>
   <si>
     <t>MESH:C104457</t>
@@ -471,6 +540,9 @@
   </si>
   <si>
     <t>https://crowdflower.com/jobs/767262/units/773932263</t>
+  </si>
+  <si>
+    <t>UNASSIGNED: Epidemiological studies of 1,3-butadiene have suggest that exposures to humans are associated with chronic myeloid leukemia (CML).</t>
   </si>
 </sst>
 </file>
@@ -599,22 +671,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:S41"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O8" activeCellId="0" sqref="O8"/>
+      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="14.9030612244898"/>
-    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.1020408163265"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.9081632653061"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.0459183673469"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.1275510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.9030612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5612244897959"/>
+    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.6734693877551"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="16" min="12" style="0" width="8.6734693877551"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.9132653061225"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.8367346938776"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="14.5867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.6734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -651,17 +725,29 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -669,10 +755,10 @@
         <v>733189</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0</v>
@@ -690,25 +776,31 @@
         <v>4</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L2" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N2" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" s="0" t="s">
-        <v>21</v>
+      <c r="O2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -716,10 +808,10 @@
         <v>920167</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0</v>
@@ -737,25 +829,34 @@
         <v>5</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="L3" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" s="0" t="s">
-        <v>28</v>
+        <v>1</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -763,10 +864,10 @@
         <v>1289188</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>0</v>
@@ -784,13 +885,13 @@
         <v>5</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L4" s="0" t="n">
         <v>1</v>
@@ -798,11 +899,20 @@
       <c r="M4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="N4" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O4" s="0" t="s">
-        <v>33</v>
+      <c r="O4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -810,10 +920,10 @@
         <v>1289188</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>0</v>
@@ -831,13 +941,13 @@
         <v>5</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L5" s="0" t="n">
         <v>1</v>
@@ -845,11 +955,20 @@
       <c r="M5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="N5" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O5" s="0" t="s">
-        <v>33</v>
+      <c r="O5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="R5" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="S5" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -857,10 +976,10 @@
         <v>1905439</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>0</v>
@@ -878,13 +997,13 @@
         <v>5</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L6" s="0" t="n">
         <v>0</v>
@@ -892,11 +1011,20 @@
       <c r="M6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N6" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="O6" s="0" t="s">
-        <v>40</v>
+      <c r="O6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="R6" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="S6" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -904,10 +1032,10 @@
         <v>2553470</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>0</v>
@@ -925,25 +1053,34 @@
         <v>5</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L7" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N7" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O7" s="0" t="s">
-        <v>45</v>
+      <c r="O7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="R7" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -951,10 +1088,10 @@
         <v>2553470</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>0</v>
@@ -972,25 +1109,31 @@
         <v>5</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L8" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N8" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O8" s="0" t="s">
-        <v>45</v>
+      <c r="O8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R8" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="S8" s="0" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -998,10 +1141,10 @@
         <v>2553470</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>0</v>
@@ -1019,25 +1162,31 @@
         <v>5</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L9" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N9" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O9" s="0" t="s">
-        <v>45</v>
+      <c r="O9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R9" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="S9" s="0" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1045,10 +1194,10 @@
         <v>2553470</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>0</v>
@@ -1066,25 +1215,34 @@
         <v>5</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L10" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N10" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O10" s="0" t="s">
-        <v>45</v>
+      <c r="O10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="R10" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="S10" s="0" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1092,10 +1250,10 @@
         <v>3109094</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>0</v>
@@ -1113,13 +1271,13 @@
         <v>5</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="L11" s="0" t="n">
         <v>1</v>
@@ -1127,11 +1285,17 @@
       <c r="M11" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="N11" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O11" s="0" t="s">
-        <v>52</v>
+      <c r="O11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R11" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="S11" s="0" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1139,10 +1303,10 @@
         <v>3538855</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>0</v>
@@ -1160,13 +1324,13 @@
         <v>5</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L12" s="0" t="n">
         <v>1</v>
@@ -1174,11 +1338,20 @@
       <c r="M12" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="N12" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O12" s="0" t="s">
-        <v>56</v>
+      <c r="O12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="R12" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="S12" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1186,10 +1359,10 @@
         <v>3895875</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>0</v>
@@ -1207,25 +1380,34 @@
         <v>5</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L13" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="N13" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="O13" s="0" t="s">
-        <v>62</v>
+      <c r="O13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="R13" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="S13" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1233,10 +1415,10 @@
         <v>7173007</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>0</v>
@@ -1254,25 +1436,37 @@
         <v>5</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="L14" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="O14" s="0" t="s">
-        <v>69</v>
+        <v>1</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="R14" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="S14" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1280,10 +1474,10 @@
         <v>8308951</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>0</v>
@@ -1301,25 +1495,31 @@
         <v>5</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="L15" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N15" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="O15" s="0" t="s">
-        <v>73</v>
+        <v>1</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="S15" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1327,10 +1527,10 @@
         <v>9759693</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>0</v>
@@ -1348,25 +1548,37 @@
         <v>5</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L16" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N16" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="O16" s="0" t="s">
-        <v>78</v>
+        <v>1</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="R16" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="S16" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1374,10 +1586,10 @@
         <v>9759693</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>0</v>
@@ -1395,25 +1607,37 @@
         <v>5</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N17" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="O17" s="0" t="s">
-        <v>78</v>
+        <v>1</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="R17" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="S17" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1421,10 +1645,10 @@
         <v>10939760</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>0</v>
@@ -1442,25 +1666,34 @@
         <v>5</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L18" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N18" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O18" s="0" t="s">
-        <v>85</v>
+        <v>1</v>
+      </c>
+      <c r="N18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R18" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="S18" s="0" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1468,10 +1701,10 @@
         <v>11380496</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>0</v>
@@ -1489,13 +1722,13 @@
         <v>5</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L19" s="0" t="n">
         <v>0</v>
@@ -1503,11 +1736,20 @@
       <c r="M19" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N19" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="O19" s="0" t="s">
-        <v>90</v>
+      <c r="O19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="R19" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="S19" s="0" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1515,10 +1757,10 @@
         <v>11380496</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>0</v>
@@ -1536,13 +1778,13 @@
         <v>5</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L20" s="0" t="n">
         <v>0</v>
@@ -1550,11 +1792,17 @@
       <c r="M20" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N20" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="O20" s="0" t="s">
-        <v>90</v>
+      <c r="O20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R20" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="S20" s="0" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1562,10 +1810,10 @@
         <v>11380496</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>0</v>
@@ -1583,13 +1831,13 @@
         <v>5</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L21" s="0" t="n">
         <v>0</v>
@@ -1597,11 +1845,20 @@
       <c r="M21" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N21" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="O21" s="0" t="s">
-        <v>90</v>
+      <c r="O21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="R21" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="S21" s="0" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1609,10 +1866,10 @@
         <v>11380496</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>0</v>
@@ -1630,13 +1887,13 @@
         <v>5</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L22" s="0" t="n">
         <v>0</v>
@@ -1644,11 +1901,20 @@
       <c r="M22" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N22" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="O22" s="0" t="s">
-        <v>90</v>
+      <c r="O22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="R22" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="S22" s="0" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1656,10 +1922,10 @@
         <v>12359538</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>0</v>
@@ -1677,25 +1943,37 @@
         <v>5</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L23" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N23" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O23" s="0" t="s">
-        <v>98</v>
+        <v>1</v>
+      </c>
+      <c r="N23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="R23" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="S23" s="0" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1703,10 +1981,10 @@
         <v>12359538</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>0</v>
@@ -1724,25 +2002,37 @@
         <v>5</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L24" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N24" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O24" s="0" t="s">
-        <v>98</v>
+        <v>1</v>
+      </c>
+      <c r="N24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="R24" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="S24" s="0" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1750,10 +2040,10 @@
         <v>12359538</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>0</v>
@@ -1771,25 +2061,37 @@
         <v>5</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L25" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N25" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O25" s="0" t="s">
-        <v>98</v>
+        <v>1</v>
+      </c>
+      <c r="N25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="R25" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="S25" s="0" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1797,10 +2099,10 @@
         <v>12359538</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>0</v>
@@ -1818,25 +2120,37 @@
         <v>5</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L26" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N26" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O26" s="0" t="s">
-        <v>98</v>
+        <v>1</v>
+      </c>
+      <c r="N26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="R26" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="S26" s="0" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1844,10 +2158,10 @@
         <v>12523489</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>0</v>
@@ -1865,25 +2179,34 @@
         <v>5</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="L27" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N27" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="O27" s="0" t="s">
-        <v>104</v>
+        <v>1</v>
+      </c>
+      <c r="N27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R27" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="S27" s="0" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1891,10 +2214,10 @@
         <v>12828076</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>0</v>
@@ -1912,13 +2235,13 @@
         <v>4</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L28" s="0" t="n">
         <v>0</v>
@@ -1926,11 +2249,20 @@
       <c r="M28" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N28" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="O28" s="0" t="s">
-        <v>109</v>
+      <c r="O28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="R28" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="S28" s="0" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1938,10 +2270,10 @@
         <v>12828076</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>0</v>
@@ -1959,13 +2291,13 @@
         <v>4</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L29" s="0" t="n">
         <v>0</v>
@@ -1973,11 +2305,20 @@
       <c r="M29" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N29" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="O29" s="0" t="s">
-        <v>109</v>
+      <c r="O29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="R29" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="S29" s="0" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1985,10 +2326,10 @@
         <v>16801510</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>0</v>
@@ -2006,25 +2347,37 @@
         <v>5</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>113</v>
+        <v>132</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="K30" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L30" s="0" t="n">
         <v>1</v>
       </c>
       <c r="M30" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N30" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="O30" s="0" t="s">
-        <v>115</v>
+        <v>0</v>
+      </c>
+      <c r="N30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="R30" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="S30" s="0" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2032,10 +2385,10 @@
         <v>17035713</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>0</v>
@@ -2053,25 +2406,31 @@
         <v>4</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>118</v>
+        <v>139</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>119</v>
+        <v>140</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L31" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M31" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N31" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="O31" s="0" t="s">
-        <v>120</v>
+      <c r="O31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R31" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="S31" s="0" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2079,10 +2438,10 @@
         <v>17035713</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>0</v>
@@ -2100,25 +2459,31 @@
         <v>4</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>118</v>
+        <v>139</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>121</v>
+        <v>143</v>
       </c>
       <c r="K32" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L32" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M32" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N32" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="O32" s="0" t="s">
-        <v>120</v>
+      <c r="O32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R32" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="S32" s="0" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2126,10 +2491,10 @@
         <v>19681452</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>0</v>
@@ -2147,25 +2512,37 @@
         <v>5</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>124</v>
+        <v>146</v>
       </c>
       <c r="K33" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L33" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M33" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N33" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="O33" s="0" t="s">
-        <v>125</v>
+        <v>1</v>
+      </c>
+      <c r="N33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="R33" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="S33" s="0" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2173,10 +2550,10 @@
         <v>24309294</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>0</v>
@@ -2194,25 +2571,34 @@
         <v>5</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="K34" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="L34" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M34" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N34" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O34" s="0" t="s">
-        <v>129</v>
+        <v>1</v>
+      </c>
+      <c r="N34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R34" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="S34" s="0" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2220,10 +2606,10 @@
         <v>24618873</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>0</v>
@@ -2241,25 +2627,34 @@
         <v>5</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>132</v>
+        <v>155</v>
       </c>
       <c r="K35" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L35" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M35" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N35" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="O35" s="0" t="s">
-        <v>133</v>
+        <v>1</v>
+      </c>
+      <c r="N35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R35" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="S35" s="0" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2267,10 +2662,10 @@
         <v>24664478</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>134</v>
+        <v>157</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>135</v>
+        <v>158</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>0</v>
@@ -2288,25 +2683,34 @@
         <v>5</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>136</v>
+        <v>159</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="K36" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L36" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M36" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N36" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O36" s="0" t="s">
-        <v>138</v>
+        <v>1</v>
+      </c>
+      <c r="N36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R36" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="S36" s="0" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2314,10 +2718,10 @@
         <v>24664478</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>134</v>
+        <v>157</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>135</v>
+        <v>158</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>0</v>
@@ -2335,25 +2739,34 @@
         <v>5</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>136</v>
+        <v>159</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>139</v>
+        <v>162</v>
       </c>
       <c r="K37" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L37" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M37" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N37" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O37" s="0" t="s">
-        <v>138</v>
+        <v>1</v>
+      </c>
+      <c r="N37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R37" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="S37" s="0" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2361,10 +2774,10 @@
         <v>24664478</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>134</v>
+        <v>157</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>135</v>
+        <v>158</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>0</v>
@@ -2382,25 +2795,34 @@
         <v>5</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>136</v>
+        <v>159</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="K38" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L38" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M38" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N38" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O38" s="0" t="s">
-        <v>138</v>
+        <v>1</v>
+      </c>
+      <c r="N38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R38" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="S38" s="0" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2408,10 +2830,10 @@
         <v>25071004</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>141</v>
+        <v>164</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>0</v>
@@ -2429,25 +2851,34 @@
         <v>4</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>143</v>
+        <v>166</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>144</v>
+        <v>167</v>
       </c>
       <c r="K39" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L39" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M39" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N39" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O39" s="0" t="s">
-        <v>145</v>
+        <v>1</v>
+      </c>
+      <c r="N39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R39" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="S39" s="0" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2455,10 +2886,10 @@
         <v>26002693</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>0</v>
@@ -2476,25 +2907,34 @@
         <v>4</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>148</v>
+        <v>171</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>149</v>
+        <v>172</v>
       </c>
       <c r="K40" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L40" s="0" t="n">
         <v>1</v>
       </c>
       <c r="M40" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N40" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="O40" s="0" t="s">
-        <v>150</v>
+        <v>0</v>
+      </c>
+      <c r="N40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R40" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="S40" s="0" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2502,10 +2942,10 @@
         <v>26002693</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>0</v>
@@ -2523,25 +2963,37 @@
         <v>4</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>148</v>
+        <v>171</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>151</v>
+        <v>174</v>
       </c>
       <c r="K41" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L41" s="0" t="n">
         <v>1</v>
       </c>
       <c r="M41" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N41" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="O41" s="0" t="s">
-        <v>150</v>
+        <v>0</v>
+      </c>
+      <c r="N41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q41" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="R41" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="S41" s="0" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>